<commit_message>
WIP for scenarios and added questions file
</commit_message>
<xml_diff>
--- a/documentation/template scénarios.xlsx
+++ b/documentation/template scénarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\2020\1er annee\Modules I-CT\I-CT 431\bataille navale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylvain.LECHAIRE\Desktop\fichiers\git\projetWeb\projetWebProvisoir\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Identifiant + Titre</t>
   </si>
@@ -48,6 +48,42 @@
   </si>
   <si>
     <t>Condition Particulière</t>
+  </si>
+  <si>
+    <t>utilisateur/acheteur potentiel</t>
+  </si>
+  <si>
+    <t>m'informer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M </t>
+  </si>
+  <si>
+    <t>PW-0001</t>
+  </si>
+  <si>
+    <t>je tappe l'url dans la barre de mon navigateur internet</t>
+  </si>
+  <si>
+    <t>naviguer sur le site internet</t>
+  </si>
+  <si>
+    <t>le serveur répond et envoye la page index.php a l'utilisateur</t>
+  </si>
+  <si>
+    <t>je clique sur un tank qui m'intéresse</t>
+  </si>
+  <si>
+    <t>une erreur quelconque se produit  côté site web/serveur</t>
+  </si>
+  <si>
+    <t>le serveur affiche une page d'erreur comme quoi la ressource demandée n'as pas pu être chargée et envoyée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je clique sur un autre tank qui m'intéresse </t>
+  </si>
+  <si>
+    <t>le serveur répond, charge et envoye la ressource demand</t>
   </si>
 </sst>
 </file>
@@ -608,13 +644,14 @@
   <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="99.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,31 +659,41 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -661,19 +708,33 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>

</xml_diff>